<commit_message>
Ender Hoppers and Droppers and all other player dependent things now work if the player is only, regardless of the dimension. Made Private chest a bit more unbreakable
</commit_message>
<xml_diff>
--- a/raw/UpgradeableTrinketsData.xlsx
+++ b/raw/UpgradeableTrinketsData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE313A4-4D98-4C23-B54F-257776D21D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841E1A36-534C-471E-AA60-3D7200212367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
+    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trinkets" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Ink</t>
   </si>
@@ -52,12 +52,21 @@
   <si>
     <t>Extra Dike (Amulet)</t>
   </si>
+  <si>
+    <t>PINK</t>
+  </si>
+  <si>
+    <t>LIGHT_BLUE</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +77,12 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -107,6 +122,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -421,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF9EA23-9E22-46CD-B6E6-BBFB5BFFD2B1}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4">
         <v>0</v>
       </c>
@@ -462,16 +478,16 @@
         <v>#NUM!</v>
       </c>
       <c r="D2" s="4" t="e">
-        <f t="shared" ref="D2:E5" si="1">1+LOG(B2/100,64)</f>
+        <f t="shared" ref="D2:D5" si="1">1+LOG(B2/100,64)</f>
         <v>#NUM!</v>
       </c>
       <c r="E2" s="4" t="e">
-        <f t="shared" ref="E2:E5" si="2">1+LOG(B2/100,32)</f>
+        <f t="shared" ref="E2" si="2">1+LOG(B2/100,32)</f>
         <v>#NUM!</v>
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -489,7 +505,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>8</v>
       </c>
@@ -507,7 +523,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>64</v>
       </c>
@@ -526,482 +542,495 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <f>100*POWER(8,A6)</f>
-        <v>100</v>
-      </c>
-      <c r="C6">
-        <f>2+LOG(B6/100,8)*2</f>
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <f>1+LOG(B6/100,32)</f>
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <f>2+LOG(B6/100,8)</f>
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <f>B6/100/64</f>
-        <v>1.5625E-2</v>
-      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <f>100*POWER(8,A7)</f>
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <f>2+LOG(B7/100,8)*2</f>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f>1+LOG(B7/100,32)</f>
         <v>1</v>
       </c>
-      <c r="B7">
-        <f t="shared" ref="B7:B25" si="5">100*POWER(8,A7)</f>
-        <v>800</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ref="C7:C24" si="6">2+LOG(B7/100,8)*2</f>
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <f t="shared" ref="D7:E24" si="7">1+LOG(B7/100,64)</f>
-        <v>1.5</v>
-      </c>
       <c r="E7">
-        <f t="shared" ref="E7:E24" si="8">2+LOG(B7/100,8)</f>
-        <v>3</v>
+        <f>2+LOG(B7/100,8)</f>
+        <v>2</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F24" si="9">B7/100/64</f>
-        <v>0.125</v>
+        <f>B7/100/64</f>
+        <v>1.5625E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <f t="shared" si="5"/>
-        <v>6400</v>
+        <f t="shared" ref="B8:B25" si="5">100*POWER(8,A8)</f>
+        <v>800</v>
       </c>
       <c r="C8">
-        <f t="shared" si="6"/>
-        <v>6</v>
+        <f t="shared" ref="C8:C25" si="6">2+LOG(B8/100,8)*2</f>
+        <v>4</v>
       </c>
       <c r="D8">
-        <f t="shared" si="7"/>
-        <v>2</v>
+        <f t="shared" ref="D8:D25" si="7">1+LOG(B8/100,64)</f>
+        <v>1.5</v>
       </c>
       <c r="E8">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f t="shared" ref="E8:E25" si="8">2+LOG(B8/100,8)</f>
+        <v>3</v>
       </c>
       <c r="F8">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <f t="shared" ref="F8:F25" si="9">B8/100/64</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <f t="shared" si="5"/>
-        <v>51200</v>
+        <v>6400</v>
       </c>
       <c r="C9">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <f t="shared" si="7"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <f t="shared" si="9"/>
-        <v>8</v>
-      </c>
-      <c r="J9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <f t="shared" si="5"/>
-        <v>409600</v>
+        <v>51200</v>
       </c>
       <c r="C10">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E10">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F10">
         <f t="shared" si="9"/>
-        <v>64</v>
-      </c>
-      <c r="J10">
-        <v>9.2233720368547697E+18</v>
+        <v>8</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <f t="shared" si="5"/>
-        <v>3276800</v>
+        <v>409600</v>
       </c>
       <c r="C11">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <f t="shared" si="7"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11">
         <f t="shared" si="9"/>
-        <v>512</v>
+        <v>64</v>
+      </c>
+      <c r="J11">
+        <v>9.2233720368547697E+18</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
         <f t="shared" si="5"/>
-        <v>26214400</v>
+        <v>3276800</v>
       </c>
       <c r="C12">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="E12">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12">
         <f t="shared" si="9"/>
-        <v>4096</v>
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <f t="shared" si="5"/>
-        <v>209715200</v>
+        <v>26214400</v>
       </c>
       <c r="C13">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <f t="shared" si="7"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <f t="shared" si="9"/>
-        <v>32768</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <f t="shared" si="5"/>
-        <v>1677721600</v>
+        <v>209715200</v>
       </c>
       <c r="C14">
         <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="D14" s="2">
-        <f t="shared" si="7"/>
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
       </c>
       <c r="E14">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <f t="shared" si="9"/>
-        <v>262144</v>
+        <v>32768</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <f t="shared" si="5"/>
-        <v>13421772800</v>
-      </c>
-      <c r="C15" s="2">
-        <f t="shared" si="6"/>
-        <v>20.000000000000004</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="7"/>
-        <v>5.5000000000000009</v>
+        <v>1677721600</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
       </c>
       <c r="E15">
         <f t="shared" si="8"/>
-        <v>11.000000000000002</v>
+        <v>10</v>
       </c>
       <c r="F15">
         <f t="shared" si="9"/>
-        <v>2097152</v>
+        <v>262144</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <f t="shared" si="5"/>
-        <v>107374182400</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="6"/>
-        <v>22</v>
+        <v>13421772800</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="6"/>
+        <v>20.000000000000004</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>5.5000000000000009</v>
       </c>
       <c r="E16">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>11.000000000000002</v>
       </c>
       <c r="F16">
         <f t="shared" si="9"/>
-        <v>16777216</v>
+        <v>2097152</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <f t="shared" si="5"/>
-        <v>858993459200</v>
+        <v>107374182400</v>
       </c>
       <c r="C17">
         <f t="shared" si="6"/>
-        <v>24.000000000000004</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>6.5000000000000009</v>
+        <v>6</v>
       </c>
       <c r="E17">
         <f t="shared" si="8"/>
-        <v>13.000000000000002</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <f t="shared" si="9"/>
-        <v>134217728</v>
+        <v>16777216</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <f t="shared" si="5"/>
-        <v>6871947673600</v>
+        <v>858993459200</v>
       </c>
       <c r="C18">
         <f t="shared" si="6"/>
-        <v>26</v>
+        <v>24.000000000000004</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>6.5000000000000009</v>
       </c>
       <c r="E18">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>13.000000000000002</v>
       </c>
       <c r="F18">
         <f t="shared" si="9"/>
-        <v>1073741824</v>
+        <v>134217728</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <f t="shared" si="5"/>
-        <v>54975581388800</v>
+        <v>6871947673600</v>
       </c>
       <c r="C19">
         <f t="shared" si="6"/>
-        <v>28.000000000000004</v>
+        <v>26</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>7.5000000000000009</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <f t="shared" si="8"/>
-        <v>15.000000000000002</v>
+        <v>14</v>
       </c>
       <c r="F19">
         <f t="shared" si="9"/>
-        <v>8589934592</v>
+        <v>1073741824</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <f t="shared" si="5"/>
-        <v>439804651110400</v>
+        <v>54975581388800</v>
       </c>
       <c r="C20">
         <f t="shared" si="6"/>
-        <v>30.000000000000004</v>
+        <v>28.000000000000004</v>
       </c>
       <c r="D20">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>7.5000000000000009</v>
       </c>
       <c r="E20">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>15.000000000000002</v>
       </c>
       <c r="F20">
         <f t="shared" si="9"/>
-        <v>68719476736</v>
+        <v>8589934592</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <f t="shared" si="5"/>
-        <v>3518437208883200</v>
+        <v>439804651110400</v>
       </c>
       <c r="C21">
         <f t="shared" si="6"/>
-        <v>32</v>
+        <v>30.000000000000004</v>
       </c>
       <c r="D21">
         <f t="shared" si="7"/>
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <f t="shared" si="9"/>
-        <v>549755813888</v>
+        <v>68719476736</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22">
         <f t="shared" si="5"/>
-        <v>2.81474976710656E+16</v>
+        <v>3518437208883200</v>
       </c>
       <c r="C22">
         <f t="shared" si="6"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="E22">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F22">
         <f t="shared" si="9"/>
-        <v>4398046511104</v>
+        <v>549755813888</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23">
         <f t="shared" si="5"/>
-        <v>2.251799813685248E+17</v>
+        <v>2.81474976710656E+16</v>
       </c>
       <c r="C23">
         <f t="shared" si="6"/>
-        <v>36.000000000000007</v>
+        <v>34</v>
       </c>
       <c r="D23">
         <f t="shared" si="7"/>
-        <v>9.5000000000000018</v>
+        <v>9</v>
       </c>
       <c r="E23">
         <f t="shared" si="8"/>
-        <v>19.000000000000004</v>
+        <v>18</v>
       </c>
       <c r="F23">
         <f t="shared" si="9"/>
-        <v>35184372088832</v>
+        <v>4398046511104</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="5"/>
+        <v>2.251799813685248E+17</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="6"/>
+        <v>36.000000000000007</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="7"/>
+        <v>9.5000000000000018</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="8"/>
+        <v>19.000000000000004</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="9"/>
+        <v>35184372088832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>18</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f t="shared" si="5"/>
         <v>1.8014398509481984E+18</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <f t="shared" si="6"/>
         <v>38.000000000000007</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D25" s="3">
         <f t="shared" si="7"/>
         <v>10.000000000000002</v>
       </c>
-      <c r="E24">
+      <c r="E25" s="2">
         <f t="shared" si="8"/>
         <v>20.000000000000004</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <f t="shared" si="9"/>
         <v>281474976710656</v>
       </c>

</xml_diff>

<commit_message>
some new wip items
</commit_message>
<xml_diff>
--- a/raw/UpgradeableTrinketsData.xlsx
+++ b/raw/UpgradeableTrinketsData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841E1A36-534C-471E-AA60-3D7200212367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF02F694-889D-49AD-8072-01E34C2CDB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Ink</t>
   </si>
@@ -60,6 +52,12 @@
   </si>
   <si>
     <t>BLUE</t>
+  </si>
+  <si>
+    <t>MAGENTA</t>
+  </si>
+  <si>
+    <t>Dig Speed Mod (Ring)</t>
   </si>
 </sst>
 </file>
@@ -440,7 +438,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +446,8 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -466,6 +465,9 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -482,10 +484,14 @@
         <v>#NUM!</v>
       </c>
       <c r="E2" s="4" t="e">
-        <f t="shared" ref="E2" si="2">1+LOG(B2/100,32)</f>
+        <f t="shared" ref="E2:F2" si="2">1+LOG(B2/100,32)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
@@ -500,10 +506,14 @@
         <v>-0.10730936496245413</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E5" si="4">2+LOG(B3/100,8)</f>
+        <f t="shared" ref="E3:F5" si="4">2+LOG(B3/100,8)</f>
         <v>-0.21461872992490827</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
@@ -521,7 +531,11 @@
         <f t="shared" si="4"/>
         <v>0.78538127007509151</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
@@ -539,7 +553,11 @@
         <f t="shared" si="4"/>
         <v>1.7853812700750917</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4">
+        <f t="shared" si="4"/>
+        <v>-0.48429787753238518</v>
+      </c>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -552,7 +570,10 @@
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -575,6 +596,10 @@
         <v>2</v>
       </c>
       <c r="F7">
+        <f>1.1 + 0.1 * LOG(B7/100,8)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G7">
         <f>B7/100/64</f>
         <v>1.5625E-2</v>
       </c>
@@ -596,11 +621,15 @@
         <v>1.5</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E25" si="8">2+LOG(B8/100,8)</f>
+        <f t="shared" ref="E8:F25" si="8">2+LOG(B8/100,8)</f>
         <v>3</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F25" si="9">B8/100/64</f>
+        <f t="shared" ref="F8:F17" si="9">1.1 + 0.1 * LOG(B8/100,8)</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="G8">
+        <f>B8/100/64</f>
         <v>0.125</v>
       </c>
     </row>
@@ -626,6 +655,10 @@
       </c>
       <c r="F9">
         <f t="shared" si="9"/>
+        <v>1.3</v>
+      </c>
+      <c r="G9">
+        <f>B9/100/64</f>
         <v>1</v>
       </c>
     </row>
@@ -651,6 +684,10 @@
       </c>
       <c r="F10">
         <f t="shared" si="9"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="G10">
+        <f>B10/100/64</f>
         <v>8</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -679,6 +716,10 @@
       </c>
       <c r="F11">
         <f t="shared" si="9"/>
+        <v>1.5</v>
+      </c>
+      <c r="G11">
+        <f>B11/100/64</f>
         <v>64</v>
       </c>
       <c r="J11">
@@ -707,6 +748,10 @@
       </c>
       <c r="F12">
         <f t="shared" si="9"/>
+        <v>1.6</v>
+      </c>
+      <c r="G12">
+        <f>B12/100/64</f>
         <v>512</v>
       </c>
     </row>
@@ -732,6 +777,10 @@
       </c>
       <c r="F13">
         <f t="shared" si="9"/>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="G13">
+        <f>B13/100/64</f>
         <v>4096</v>
       </c>
     </row>
@@ -757,6 +806,10 @@
       </c>
       <c r="F14">
         <f t="shared" si="9"/>
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="G14">
+        <f>B14/100/64</f>
         <v>32768</v>
       </c>
     </row>
@@ -782,6 +835,10 @@
       </c>
       <c r="F15">
         <f t="shared" si="9"/>
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="G15">
+        <f>B15/100/64</f>
         <v>262144</v>
       </c>
     </row>
@@ -805,12 +862,16 @@
         <f t="shared" si="8"/>
         <v>11.000000000000002</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <f t="shared" si="9"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="G16">
+        <f>B16/100/64</f>
         <v>2097152</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -830,12 +891,12 @@
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="9"/>
+      <c r="G17">
+        <f>B17/100/64</f>
         <v>16777216</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -855,12 +916,12 @@
         <f t="shared" si="8"/>
         <v>13.000000000000002</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="9"/>
+      <c r="G18">
+        <f>B18/100/64</f>
         <v>134217728</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -880,12 +941,12 @@
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="9"/>
+      <c r="G19">
+        <f>B19/100/64</f>
         <v>1073741824</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -905,12 +966,12 @@
         <f t="shared" si="8"/>
         <v>15.000000000000002</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="9"/>
+      <c r="G20">
+        <f>B20/100/64</f>
         <v>8589934592</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
@@ -930,12 +991,12 @@
         <f t="shared" si="8"/>
         <v>16</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="9"/>
+      <c r="G21">
+        <f>B21/100/64</f>
         <v>68719476736</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
@@ -955,12 +1016,12 @@
         <f t="shared" si="8"/>
         <v>17</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="9"/>
+      <c r="G22">
+        <f>B22/100/64</f>
         <v>549755813888</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16</v>
       </c>
@@ -980,12 +1041,12 @@
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="9"/>
+      <c r="G23">
+        <f>B23/100/64</f>
         <v>4398046511104</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17</v>
       </c>
@@ -1005,12 +1066,12 @@
         <f t="shared" si="8"/>
         <v>19.000000000000004</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="9"/>
+      <c r="G24">
+        <f>B24/100/64</f>
         <v>35184372088832</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
@@ -1030,8 +1091,8 @@
         <f t="shared" si="8"/>
         <v>20.000000000000004</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="9"/>
+      <c r="G25">
+        <f>B25/100/64</f>
         <v>281474976710656</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added malachite items. Rendering mostly works (crossbow still missing)
</commit_message>
<xml_diff>
--- a/raw/UpgradeableTrinketsData.xlsx
+++ b/raw/UpgradeableTrinketsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF02F694-889D-49AD-8072-01E34C2CDB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD7E82C-944F-467C-93FA-58D00F48DF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
+    <workbookView xWindow="23355" yWindow="0" windowWidth="28245" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trinkets" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Ink</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Dig Speed Mod (Ring)</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>Extra Crit Damage (Ring)</t>
+  </si>
+  <si>
+    <t>Villager Discount</t>
+  </si>
+  <si>
+    <t>GREEN</t>
   </si>
 </sst>
 </file>
@@ -112,13 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -435,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF9EA23-9E22-46CD-B6E6-BBFB5BFFD2B1}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,11 +458,13 @@
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -468,114 +481,134 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="e">
+      <c r="C2" s="3" t="e">
         <f t="shared" ref="C2" si="0">1+LOG(B2/100,8)</f>
         <v>#NUM!</v>
       </c>
-      <c r="D2" s="4" t="e">
+      <c r="D2" s="3" t="e">
         <f t="shared" ref="D2:D5" si="1">1+LOG(B2/100,64)</f>
         <v>#NUM!</v>
       </c>
-      <c r="E2" s="4" t="e">
+      <c r="E2" s="3" t="e">
         <f t="shared" ref="E2:F2" si="2">1+LOG(B2/100,32)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F2" s="4" t="e">
+      <c r="F2" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <f t="shared" ref="C3:C5" si="3">1+LOG(B3/100,8)*2</f>
         <v>-3.4292374598498165</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f t="shared" si="1"/>
         <v>-0.10730936496245413</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f t="shared" ref="E3:F5" si="4">2+LOG(B3/100,8)</f>
         <v>-0.21461872992490827</v>
       </c>
-      <c r="F3" s="4" t="e">
+      <c r="F3" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <f t="shared" si="3"/>
         <v>-1.429237459849817</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f t="shared" si="1"/>
         <v>0.39269063503754575</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <f t="shared" si="4"/>
         <v>0.78538127007509151</v>
       </c>
-      <c r="F4" s="4" t="e">
+      <c r="F4" s="3" t="e">
         <f t="shared" si="4"/>
         <v>#NUM!</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>64</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <f t="shared" si="3"/>
         <v>0.57076254015018346</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" si="1"/>
         <v>0.89269063503754587</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f t="shared" si="4"/>
         <v>1.7853812700750917</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f t="shared" si="4"/>
         <v>-0.48429787753238518</v>
       </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -588,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <f>1+LOG(B7/100,32)</f>
+        <f>1+LOG(B7/100,64)</f>
         <v>1</v>
       </c>
       <c r="E7">
@@ -600,499 +633,499 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G7">
-        <f>B7/100/64</f>
+        <f>1+LOG(B7/100,64)</f>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f>1+2*LOG(B7/100,64)</f>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I25" si="5">B7/100/64</f>
         <v>1.5625E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B25" si="5">100*POWER(8,A8)</f>
+        <f t="shared" ref="B8:B25" si="6">100*POWER(8,A8)</f>
         <v>800</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C25" si="6">2+LOG(B8/100,8)*2</f>
+        <f t="shared" ref="C8:C16" si="7">2+LOG(B8/100,8)*2</f>
         <v>4</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D25" si="7">1+LOG(B8/100,64)</f>
+        <f t="shared" ref="D8:D15" si="8">1+LOG(B8/100,64)</f>
         <v>1.5</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:F25" si="8">2+LOG(B8/100,8)</f>
+        <f t="shared" ref="E8:E25" si="9">2+LOG(B8/100,8)</f>
         <v>3</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F17" si="9">1.1 + 0.1 * LOG(B8/100,8)</f>
+        <f t="shared" ref="F8:F16" si="10">1.1 + 0.1 * LOG(B8/100,8)</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="G8">
-        <f>B8/100/64</f>
+        <f t="shared" ref="G8:G15" si="11">1+LOG(B8/100,64)</f>
+        <v>1.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H16" si="12">1+2*LOG(B8/100,64)</f>
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6400</v>
       </c>
       <c r="C9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="D9">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="10"/>
+        <v>1.3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="6"/>
+        <v>51200</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="10"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="6"/>
+        <v>409600</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="L11">
+        <v>9.2233720368547697E+18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="6"/>
+        <v>3276800</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="8"/>
+        <v>3.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="10"/>
+        <v>1.6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="11"/>
+        <v>3.5</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="6"/>
+        <v>26214400</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="9"/>
-        <v>1.3</v>
-      </c>
-      <c r="G9">
-        <f>B9/100/64</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="5"/>
-        <v>51200</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="6"/>
+      <c r="E13">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="F13">
+        <f t="shared" si="10"/>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="6"/>
+        <v>209715200</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="7"/>
-        <v>2.5</v>
-      </c>
-      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="10"/>
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="11"/>
+        <v>4.5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="6"/>
+        <v>1677721600</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="9"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="G10">
-        <f>B10/100/64</f>
-        <v>8</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="5"/>
-        <v>409600</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="6"/>
+      <c r="E15">
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="G11">
-        <f>B11/100/64</f>
-        <v>64</v>
-      </c>
-      <c r="J11">
-        <v>9.2233720368547697E+18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="F15">
+        <f t="shared" si="10"/>
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="5"/>
-        <v>3276800</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="6"/>
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="7"/>
-        <v>3.5</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="9"/>
-        <v>1.6</v>
-      </c>
-      <c r="G12">
-        <f>B12/100/64</f>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="5"/>
-        <v>26214400</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="6"/>
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="9"/>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="G13">
-        <f>B13/100/64</f>
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="5"/>
-        <v>209715200</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="7"/>
-        <v>4.5</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="8"/>
+      <c r="H15">
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="9"/>
-        <v>1.8000000000000003</v>
-      </c>
-      <c r="G14">
-        <f>B14/100/64</f>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="5"/>
-        <v>1677721600</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="D15" s="2">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="9"/>
-        <v>1.9000000000000001</v>
-      </c>
-      <c r="G15">
-        <f>B15/100/64</f>
+      <c r="I15">
+        <f t="shared" si="5"/>
         <v>262144</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
       <c r="B16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13421772800</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>20.000000000000004</v>
       </c>
-      <c r="D16">
-        <f t="shared" si="7"/>
-        <v>5.5000000000000009</v>
-      </c>
       <c r="E16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11.000000000000002</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.0000000000000004</v>
       </c>
-      <c r="G16">
-        <f>B16/100/64</f>
+      <c r="H16" s="2">
+        <f t="shared" si="12"/>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
         <v>2097152</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="B17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>107374182400</v>
       </c>
-      <c r="C17">
-        <f t="shared" si="6"/>
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
       <c r="E17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="G17">
-        <f>B17/100/64</f>
+      <c r="I17">
+        <f t="shared" si="5"/>
         <v>16777216</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
       <c r="B18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>858993459200</v>
       </c>
-      <c r="C18">
-        <f t="shared" si="6"/>
-        <v>24.000000000000004</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="7"/>
-        <v>6.5000000000000009</v>
-      </c>
       <c r="E18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>13.000000000000002</v>
       </c>
-      <c r="G18">
-        <f>B18/100/64</f>
+      <c r="I18">
+        <f t="shared" si="5"/>
         <v>134217728</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6871947673600</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="6"/>
-        <v>26</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
       <c r="E19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="G19">
-        <f>B19/100/64</f>
+      <c r="I19">
+        <f t="shared" si="5"/>
         <v>1073741824</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
       <c r="B20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>54975581388800</v>
       </c>
-      <c r="C20">
-        <f t="shared" si="6"/>
-        <v>28.000000000000004</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="7"/>
-        <v>7.5000000000000009</v>
-      </c>
       <c r="E20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>15.000000000000002</v>
       </c>
-      <c r="G20">
-        <f>B20/100/64</f>
+      <c r="I20">
+        <f t="shared" si="5"/>
         <v>8589934592</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
       <c r="B21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>439804651110400</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="6"/>
-        <v>30.000000000000004</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
       <c r="E21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
-      <c r="G21">
-        <f>B21/100/64</f>
+      <c r="I21">
+        <f t="shared" si="5"/>
         <v>68719476736</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
       <c r="B22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3518437208883200</v>
       </c>
-      <c r="C22">
-        <f t="shared" si="6"/>
-        <v>32</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="7"/>
-        <v>8.5</v>
-      </c>
       <c r="E22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="G22">
-        <f>B22/100/64</f>
+      <c r="I22">
+        <f t="shared" si="5"/>
         <v>549755813888</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>16</v>
       </c>
       <c r="B23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.81474976710656E+16</v>
       </c>
-      <c r="C23">
-        <f t="shared" si="6"/>
-        <v>34</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
       <c r="E23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
-      <c r="G23">
-        <f>B23/100/64</f>
+      <c r="I23">
+        <f t="shared" si="5"/>
         <v>4398046511104</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>17</v>
       </c>
       <c r="B24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.251799813685248E+17</v>
       </c>
-      <c r="C24">
-        <f t="shared" si="6"/>
-        <v>36.000000000000007</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="7"/>
-        <v>9.5000000000000018</v>
-      </c>
       <c r="E24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>19.000000000000004</v>
       </c>
-      <c r="G24">
-        <f>B24/100/64</f>
+      <c r="I24">
+        <f t="shared" si="5"/>
         <v>35184372088832</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>18</v>
       </c>
       <c r="B25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.8014398509481984E+18</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="6"/>
-        <v>38.000000000000007</v>
-      </c>
-      <c r="D25" s="3">
-        <f t="shared" si="7"/>
-        <v>10.000000000000002</v>
-      </c>
       <c r="E25" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>20.000000000000004</v>
       </c>
-      <c r="G25">
-        <f>B25/100/64</f>
+      <c r="I25">
+        <f t="shared" si="5"/>
         <v>281474976710656</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unified the way upgradeable trinkets calculate their upgrade values. All now cap out at 3276800 Ink
</commit_message>
<xml_diff>
--- a/raw/UpgradeableTrinketsData.xlsx
+++ b/raw/UpgradeableTrinketsData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD7E82C-944F-467C-93FA-58D00F48DF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6848DE7-E626-4D35-9EF6-4B007DC40485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23355" yWindow="0" windowWidth="28245" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
+    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{364233D7-E848-40E5-85B2-7130C91DE93F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trinkets" sheetId="1" r:id="rId1"/>
+    <sheet name="Trinkets_deeper_down" sheetId="2" r:id="rId1"/>
+    <sheet name="Trinkets_old" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Ink</t>
   </si>
@@ -70,6 +71,12 @@
   </si>
   <si>
     <t>GREEN</t>
+  </si>
+  <si>
+    <t>&lt;-- current cap</t>
+  </si>
+  <si>
+    <t>&lt;-- endgame cap</t>
   </si>
 </sst>
 </file>
@@ -124,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -132,6 +139,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -445,11 +455,686 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A88A3B5-CA77-441F-B4E6-7188A569AE45}">
+  <dimension ref="A1:L29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="e">
+        <f t="shared" ref="C2" si="0">1+LOG(B2/100,8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D2" s="3" t="e">
+        <f t="shared" ref="D2:D5" si="1">1+LOG(B2/100,64)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="E2" s="3" t="e">
+        <f t="shared" ref="E2:F2" si="2">1+LOG(B2/100,32)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F2" s="3" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C5" si="3">1+LOG(B3/100,8)*2</f>
+        <v>-3.4292374598498165</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.10730936496245413</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:F5" si="4">2+LOG(B3/100,8)</f>
+        <v>-0.21461872992490827</v>
+      </c>
+      <c r="F3" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="3"/>
+        <v>-1.429237459849817</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39269063503754575</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="4"/>
+        <v>0.78538127007509151</v>
+      </c>
+      <c r="F4" s="3" t="e">
+        <f t="shared" si="4"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>64</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="3"/>
+        <v>0.57076254015018346</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.89269063503754587</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="4"/>
+        <v>1.7853812700750917</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.48429787753238518</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <f>100*POWER(8,A7)</f>
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <f>2+LOG(B7/100,8)*2</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <f>0.5+LOG(B7/100,64)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="4">
+        <f>1+LOG(B7/100,8)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <f>1.1 + 0.1 * LOG(B7/100,8)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G7" s="4">
+        <f>0.5+LOG(B7/100,64)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="4">
+        <f>1+2*LOG(B7/100,64)</f>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I25" si="5">B7/100/64</f>
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:B25" si="6">100*POWER(8,A8)</f>
+        <v>800</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C16" si="7">2+LOG(B8/100,8)*2</f>
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" ref="D8:D16" si="8">0.5+LOG(B8/100,64)</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" ref="E8:E16" si="9">1+LOG(B8/100,8)</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" ref="F8:F16" si="10">1.1 + 0.1 * LOG(B8/100,8)</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:G16" si="11">0.5+LOG(B8/100,64)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" ref="H8:H16" si="12">1+2*LOG(B8/100,64)</f>
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="6"/>
+        <v>6400</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="8"/>
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="10"/>
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="6"/>
+        <v>51200</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="10"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="6"/>
+        <v>409600</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="8"/>
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="11"/>
+        <v>2.5</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="L11">
+        <v>9.2233720368547697E+18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="6"/>
+        <v>3276800</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="10"/>
+        <v>1.6</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="6"/>
+        <v>26214400</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="8"/>
+        <v>3.5</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="10"/>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="11"/>
+        <v>3.5</v>
+      </c>
+      <c r="H13" s="4">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="6"/>
+        <v>209715200</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="10"/>
+        <v>1.8000000000000003</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="6"/>
+        <v>1677721600</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="10"/>
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="11"/>
+        <v>4.5</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="6"/>
+        <v>13421772800</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="7"/>
+        <v>20.000000000000004</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="8"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="9"/>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="10"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="11"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="12"/>
+        <v>10.000000000000002</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>2097152</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="6"/>
+        <v>107374182400</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="6"/>
+        <v>858993459200</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="6"/>
+        <v>6871947673600</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>1073741824</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="6"/>
+        <v>54975581388800</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>8589934592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="6"/>
+        <v>439804651110400</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>68719476736</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="6"/>
+        <v>3518437208883200</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="5"/>
+        <v>549755813888</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="6"/>
+        <v>2.81474976710656E+16</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="5"/>
+        <v>4398046511104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="6"/>
+        <v>2.251799813685248E+17</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="5"/>
+        <v>35184372088832</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="6"/>
+        <v>1.8014398509481984E+18</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="5"/>
+        <v>281474976710656</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF9EA23-9E22-46CD-B6E6-BBFB5BFFD2B1}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A1:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>